<commit_message>
change for 🕸 production and finally they work like a charm 😎
</commit_message>
<xml_diff>
--- a/studi-kasus-2/kasus/Studi-kasus2.xlsx
+++ b/studi-kasus-2/kasus/Studi-kasus2.xlsx
@@ -1077,7 +1077,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1151,7 +1151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:5">
       <c r="B6" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1160,6 +1160,9 @@
         <v>11</v>
       </c>
       <c r="D6" s="3"/>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="2">
@@ -1174,7 +1177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:5">
       <c r="B8" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1183,6 +1186,9 @@
         <v>13</v>
       </c>
       <c r="D8" s="3"/>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="2">
@@ -1199,7 +1205,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:5">
       <c r="B10" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1208,6 +1214,9 @@
         <v>16</v>
       </c>
       <c r="D10" s="3"/>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="2">

</xml_diff>